<commit_message>
updating QTL2 report code
</commit_message>
<xml_diff>
--- a/R2D2-Liver-GSH-NAD/results/QTL List LOD Score 6.xlsx
+++ b/R2D2-Liver-GSH-NAD/results/QTL List LOD Score 6.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="QTL List RankZ Sex - cM" sheetId="1" r:id="rId1"/>
     <sheet name="QTL List RankZ Sex - Mbp" sheetId="2" r:id="rId2"/>
-    <sheet name="QTL List RankZ SexGeb=n - cM" sheetId="3" r:id="rId3"/>
+    <sheet name="QTL List RankZ SexGen - cM" sheetId="3" r:id="rId3"/>
     <sheet name="QTL List RankZ SexGen - Mbp" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>JAX00357615</t>
+          <t>UNCHS035922</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>UNC3398043</t>
+          <t>UNCHS005556</t>
         </is>
       </c>
     </row>
@@ -782,7 +782,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>ICR5070</t>
+          <t>ICR1070</t>
         </is>
       </c>
     </row>
@@ -814,7 +814,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>ICR5071</t>
+          <t>JAX00096955</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>UNCHS029729</t>
+          <t>UNC19016786</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>UNCHS035922</t>
+          <t>JAX00357615</t>
         </is>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>JAX00066393</t>
+          <t>JAX00066393r</t>
         </is>
       </c>
     </row>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>UNC3398043</t>
+          <t>UNCHS005556</t>
         </is>
       </c>
     </row>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>UNC3398043</t>
+          <t>UNCHS005556</t>
         </is>
       </c>
     </row>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>UNCHS036806</t>
+          <t>UNC23135640</t>
         </is>
       </c>
     </row>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>UNCHS005556</t>
+          <t>UNC3398043</t>
         </is>
       </c>
     </row>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>JAX00066393r</t>
+          <t>JAX00066393</t>
         </is>
       </c>
     </row>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>UNCHS009831</t>
+          <t>UNCHS009832</t>
         </is>
       </c>
     </row>

</xml_diff>